<commit_message>
nuevos datos para seeds
</commit_message>
<xml_diff>
--- a/src/utils/csv/BBDD_BonoBooking.xlsx
+++ b/src/utils/csv/BBDD_BonoBooking.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28025"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://meliao365-my.sharepoint.com/personal/ana_maria_rodriguez_melia_com/Documents/Escritorio/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="85" documentId="11_F4E994B0186C0E6FD7667E7E74E447CA570E4C2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{14A9B21C-E0BC-4AE9-9CD1-932F93599C29}"/>
+  <xr:revisionPtr revIDLastSave="150" documentId="11_F4E994B0186C0E6FD7667E7E74E447CA570E4C2A" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{8FACFD25-367C-47B8-91F5-AED5BD63D49B}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="17640" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-1815" windowWidth="29040" windowHeight="17640" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="users" sheetId="7" r:id="rId1"/>
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="372" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="552" uniqueCount="338">
   <si>
     <t>ID</t>
   </si>
@@ -370,9 +370,6 @@
     <t>user (ID)</t>
   </si>
   <si>
-    <t>Bono</t>
-  </si>
-  <si>
     <t>CODE001</t>
   </si>
   <si>
@@ -433,135 +430,90 @@
     <t>**************</t>
   </si>
   <si>
-    <t>[1, 2]</t>
-  </si>
-  <si>
     <t>usuario2@example.com</t>
   </si>
   <si>
     <t>user2</t>
   </si>
   <si>
-    <t>[3, 4]</t>
-  </si>
-  <si>
     <t>usuario3@example.com</t>
   </si>
   <si>
     <t>user3</t>
   </si>
   <si>
-    <t>[5, 6]</t>
-  </si>
-  <si>
     <t>usuario4@example.com</t>
   </si>
   <si>
     <t>user4</t>
   </si>
   <si>
-    <t>[7, 8]</t>
-  </si>
-  <si>
     <t>usuario5@example.com</t>
   </si>
   <si>
     <t>user5</t>
   </si>
   <si>
-    <t>[9, 10]</t>
-  </si>
-  <si>
     <t>usuario6@example.com</t>
   </si>
   <si>
     <t>user6</t>
   </si>
   <si>
-    <t>[11, 12]</t>
-  </si>
-  <si>
     <t>usuario7@example.com</t>
   </si>
   <si>
     <t>user7</t>
   </si>
   <si>
-    <t>[13, 14]</t>
-  </si>
-  <si>
     <t>usuario8@example.com</t>
   </si>
   <si>
     <t>user8</t>
   </si>
   <si>
-    <t>[15, 16]</t>
-  </si>
-  <si>
     <t>usuario9@example.com</t>
   </si>
   <si>
     <t>user9</t>
   </si>
   <si>
-    <t>[17, 18]</t>
-  </si>
-  <si>
     <t>usuario10@example.com</t>
   </si>
   <si>
     <t>user10</t>
   </si>
   <si>
-    <t>[19, 20]</t>
-  </si>
-  <si>
     <t>usuario11@example.com</t>
   </si>
   <si>
     <t>user11</t>
   </si>
   <si>
-    <t>[21, 22]</t>
-  </si>
-  <si>
     <t>usuario12@example.com</t>
   </si>
   <si>
     <t>user12</t>
   </si>
   <si>
-    <t>[23, 24]</t>
-  </si>
-  <si>
     <t>usuario13@example.com</t>
   </si>
   <si>
     <t>user13</t>
   </si>
   <si>
-    <t>[25, 26]</t>
-  </si>
-  <si>
     <t>usuario14@example.com</t>
   </si>
   <si>
     <t>user14</t>
   </si>
   <si>
-    <t>[27, 28]</t>
-  </si>
-  <si>
     <t>usuario15@example.com</t>
   </si>
   <si>
     <t>user15</t>
   </si>
   <si>
-    <t>[29, 30]</t>
-  </si>
-  <si>
     <t>usuario16@example.com</t>
   </si>
   <si>
@@ -650,13 +602,448 @@
   </si>
   <si>
     <t>user30</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c20</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c21</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c22</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c23</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c24</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c25</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c26</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c27</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c28</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c29</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c2f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c30</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c31</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c32</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c33</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c34</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c35</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c36</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c37</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c38</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c39</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c3f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c40</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c41</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c42</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c43</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c44</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c45</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c46</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c47</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c48</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c49</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c4f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c50</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c51</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c52</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c53</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c54</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c55</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c56</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c57</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c58</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c59</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c01</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c02</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c03</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c04</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c05</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c06</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c07</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c08</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c09</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c0f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c10</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c11</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c12</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c13</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c14</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c15</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c16</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c17</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c18</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c19</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c1e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c5f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c60</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c61</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c62</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c63</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c64</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c65</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c66</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c67</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c68</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c69</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6a</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6b</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6c</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6d</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6e</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c6f</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c70</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c71</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c72</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c73</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c74</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c75</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c76</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c77</t>
+  </si>
+  <si>
+    <t>618f1a2b3c4d5e6f7a8b9c78</t>
+  </si>
+  <si>
+    <t>admin</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c48]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c49]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c3e]</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c3f]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c40]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c41]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c42]</t>
+  </si>
+  <si>
+    <t>[618f1a2b3c4d5e6f7a8b9c47]</t>
+  </si>
+  <si>
+    <t>Bono 1</t>
+  </si>
+  <si>
+    <t>Bono 2</t>
+  </si>
+  <si>
+    <t>Bono 3</t>
+  </si>
+  <si>
+    <t>Bono 4</t>
+  </si>
+  <si>
+    <t>Bono 5</t>
+  </si>
+  <si>
+    <t>Bono 6</t>
+  </si>
+  <si>
+    <t>Bono 7</t>
+  </si>
+  <si>
+    <t>Bono 8</t>
+  </si>
+  <si>
+    <t>Bono 9</t>
+  </si>
+  <si>
+    <t>Bono 10</t>
+  </si>
+  <si>
+    <t>Bono 11</t>
+  </si>
+  <si>
+    <t>Bono 12</t>
+  </si>
+  <si>
+    <t>Bono 13</t>
+  </si>
+  <si>
+    <t>Bono 14</t>
+  </si>
+  <si>
+    <t>Bono 15</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="5" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -675,6 +1062,21 @@
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="Arial"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="2"/>
       <scheme val="minor"/>
     </font>
   </fonts>
@@ -699,7 +1101,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
@@ -714,6 +1116,12 @@
       <alignment vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="20" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -938,13 +1346,14 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{5F5884DD-214E-4264-8B67-7F7D32F5C2B7}">
   <dimension ref="A1:G31"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection sqref="A1:G31"/>
+    <sheetView topLeftCell="A5" workbookViewId="0">
+      <selection activeCell="G3" sqref="G3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="5" max="5" width="96" customWidth="1"/>
+    <col min="5" max="5" width="7.6328125" customWidth="1"/>
+    <col min="7" max="7" width="31.453125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:7" ht="26" x14ac:dyDescent="0.25">
@@ -961,50 +1370,50 @@
         <v>12</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>131</v>
+        <v>130</v>
       </c>
       <c r="F1" s="1" t="s">
         <v>1</v>
       </c>
       <c r="G1" s="1" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>283</v>
+      </c>
+      <c r="B2" s="2" t="s">
         <v>132</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
-      </c>
-      <c r="B2" s="2" t="s">
+      <c r="C2" s="2" t="s">
         <v>133</v>
       </c>
-      <c r="C2" s="2" t="s">
+      <c r="D2" s="2" t="s">
         <v>134</v>
       </c>
-      <c r="D2" s="2" t="s">
-        <v>135</v>
-      </c>
-      <c r="E2" s="2" t="s">
-        <v>9</v>
+      <c r="E2" s="7" t="s">
+        <v>313</v>
       </c>
       <c r="F2" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G2" s="2" t="s">
+      <c r="G2" s="7" t="s">
+        <v>314</v>
+      </c>
+    </row>
+    <row r="3" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="2" t="s">
+        <v>284</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>135</v>
+      </c>
+      <c r="C3" s="2" t="s">
         <v>136</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
-      </c>
-      <c r="B3" s="2" t="s">
-        <v>137</v>
-      </c>
-      <c r="C3" s="2" t="s">
-        <v>138</v>
-      </c>
       <c r="D3" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E3" s="2" t="s">
         <v>9</v>
@@ -1012,22 +1421,22 @@
       <c r="F3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G3" s="2" t="s">
-        <v>139</v>
+      <c r="G3" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="4" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>285</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C4" s="2" t="s">
-        <v>141</v>
+        <v>138</v>
       </c>
       <c r="D4" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E4" s="2" t="s">
         <v>9</v>
@@ -1035,22 +1444,22 @@
       <c r="F4" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G4" s="2" t="s">
-        <v>142</v>
+      <c r="G4" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="5" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>286</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>143</v>
+        <v>139</v>
       </c>
       <c r="C5" s="2" t="s">
-        <v>144</v>
+        <v>140</v>
       </c>
       <c r="D5" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E5" s="2" t="s">
         <v>9</v>
@@ -1058,22 +1467,22 @@
       <c r="F5" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G5" s="2" t="s">
-        <v>145</v>
+      <c r="G5" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="6" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>287</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>146</v>
+        <v>141</v>
       </c>
       <c r="C6" s="2" t="s">
-        <v>147</v>
+        <v>142</v>
       </c>
       <c r="D6" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E6" s="2" t="s">
         <v>9</v>
@@ -1081,22 +1490,22 @@
       <c r="F6" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G6" s="2" t="s">
-        <v>148</v>
+      <c r="G6" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="7" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
+      <c r="A7" s="2" t="s">
+        <v>288</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C7" s="2" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="D7" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E7" s="2" t="s">
         <v>9</v>
@@ -1104,22 +1513,22 @@
       <c r="F7" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G7" s="2" t="s">
-        <v>151</v>
+      <c r="G7" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="8" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
+      <c r="A8" s="2" t="s">
+        <v>289</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>152</v>
+        <v>145</v>
       </c>
       <c r="C8" s="2" t="s">
-        <v>153</v>
+        <v>146</v>
       </c>
       <c r="D8" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E8" s="2" t="s">
         <v>9</v>
@@ -1127,22 +1536,22 @@
       <c r="F8" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G8" s="2" t="s">
-        <v>154</v>
+      <c r="G8" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="9" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
+      <c r="A9" s="2" t="s">
+        <v>290</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>155</v>
+        <v>147</v>
       </c>
       <c r="C9" s="2" t="s">
-        <v>156</v>
+        <v>148</v>
       </c>
       <c r="D9" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E9" s="2" t="s">
         <v>9</v>
@@ -1150,22 +1559,22 @@
       <c r="F9" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G9" s="2" t="s">
-        <v>157</v>
+      <c r="G9" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="10" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
+      <c r="A10" s="2" t="s">
+        <v>291</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="C10" s="2" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="D10" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E10" s="2" t="s">
         <v>9</v>
@@ -1173,22 +1582,22 @@
       <c r="F10" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G10" s="2" t="s">
-        <v>160</v>
+      <c r="G10" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="11" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
+      <c r="A11" s="2" t="s">
+        <v>292</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C11" s="2" t="s">
-        <v>162</v>
+        <v>152</v>
       </c>
       <c r="D11" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E11" s="2" t="s">
         <v>9</v>
@@ -1196,22 +1605,22 @@
       <c r="F11" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G11" s="2" t="s">
-        <v>163</v>
+      <c r="G11" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="12" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
+      <c r="A12" s="2" t="s">
+        <v>293</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>164</v>
+        <v>153</v>
       </c>
       <c r="C12" s="2" t="s">
-        <v>165</v>
+        <v>154</v>
       </c>
       <c r="D12" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E12" s="2" t="s">
         <v>9</v>
@@ -1219,22 +1628,22 @@
       <c r="F12" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G12" s="2" t="s">
-        <v>166</v>
+      <c r="G12" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="13" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
+      <c r="A13" s="2" t="s">
+        <v>294</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>167</v>
+        <v>155</v>
       </c>
       <c r="C13" s="2" t="s">
-        <v>168</v>
+        <v>156</v>
       </c>
       <c r="D13" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E13" s="2" t="s">
         <v>9</v>
@@ -1242,22 +1651,22 @@
       <c r="F13" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G13" s="2" t="s">
-        <v>169</v>
+      <c r="G13" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="14" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
+      <c r="A14" s="2" t="s">
+        <v>295</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>170</v>
+        <v>157</v>
       </c>
       <c r="C14" s="2" t="s">
-        <v>171</v>
+        <v>158</v>
       </c>
       <c r="D14" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E14" s="2" t="s">
         <v>9</v>
@@ -1265,22 +1674,22 @@
       <c r="F14" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G14" s="2" t="s">
-        <v>172</v>
+      <c r="G14" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="15" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
+      <c r="A15" s="2" t="s">
+        <v>296</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>173</v>
+        <v>159</v>
       </c>
       <c r="C15" s="2" t="s">
-        <v>174</v>
+        <v>160</v>
       </c>
       <c r="D15" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E15" s="2" t="s">
         <v>9</v>
@@ -1288,22 +1697,22 @@
       <c r="F15" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G15" s="2" t="s">
-        <v>175</v>
+      <c r="G15" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="16" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
+      <c r="A16" s="2" t="s">
+        <v>297</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>176</v>
+        <v>161</v>
       </c>
       <c r="C16" s="2" t="s">
-        <v>177</v>
+        <v>162</v>
       </c>
       <c r="D16" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E16" s="2" t="s">
         <v>9</v>
@@ -1311,22 +1720,22 @@
       <c r="F16" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G16" s="2" t="s">
-        <v>178</v>
+      <c r="G16" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="17" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
+      <c r="A17" s="2" t="s">
+        <v>298</v>
       </c>
       <c r="B17" s="2" t="s">
-        <v>179</v>
+        <v>163</v>
       </c>
       <c r="C17" s="2" t="s">
-        <v>180</v>
+        <v>164</v>
       </c>
       <c r="D17" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E17" s="2" t="s">
         <v>9</v>
@@ -1334,22 +1743,22 @@
       <c r="F17" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G17" s="2" t="s">
-        <v>136</v>
+      <c r="G17" s="7" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="18" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
+      <c r="A18" s="2" t="s">
+        <v>299</v>
       </c>
       <c r="B18" s="2" t="s">
-        <v>181</v>
+        <v>165</v>
       </c>
       <c r="C18" s="2" t="s">
-        <v>182</v>
+        <v>166</v>
       </c>
       <c r="D18" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E18" s="2" t="s">
         <v>9</v>
@@ -1357,22 +1766,22 @@
       <c r="F18" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G18" s="2" t="s">
-        <v>139</v>
+      <c r="G18" s="7" t="s">
+        <v>315</v>
       </c>
     </row>
     <row r="19" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
+      <c r="A19" s="2" t="s">
+        <v>300</v>
       </c>
       <c r="B19" s="2" t="s">
-        <v>183</v>
+        <v>167</v>
       </c>
       <c r="C19" s="2" t="s">
-        <v>184</v>
+        <v>168</v>
       </c>
       <c r="D19" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E19" s="2" t="s">
         <v>9</v>
@@ -1380,22 +1789,22 @@
       <c r="F19" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G19" s="2" t="s">
-        <v>142</v>
+      <c r="G19" s="7" t="s">
+        <v>316</v>
       </c>
     </row>
     <row r="20" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
+      <c r="A20" s="2" t="s">
+        <v>301</v>
       </c>
       <c r="B20" s="2" t="s">
-        <v>185</v>
+        <v>169</v>
       </c>
       <c r="C20" s="2" t="s">
-        <v>186</v>
+        <v>170</v>
       </c>
       <c r="D20" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E20" s="2" t="s">
         <v>9</v>
@@ -1403,22 +1812,22 @@
       <c r="F20" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G20" s="2" t="s">
-        <v>145</v>
+      <c r="G20" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="21" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
+      <c r="A21" s="2" t="s">
+        <v>302</v>
       </c>
       <c r="B21" s="2" t="s">
-        <v>187</v>
+        <v>171</v>
       </c>
       <c r="C21" s="2" t="s">
-        <v>188</v>
+        <v>172</v>
       </c>
       <c r="D21" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E21" s="2" t="s">
         <v>9</v>
@@ -1426,22 +1835,22 @@
       <c r="F21" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G21" s="2" t="s">
-        <v>148</v>
+      <c r="G21" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="22" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
+      <c r="A22" s="2" t="s">
+        <v>303</v>
       </c>
       <c r="B22" s="2" t="s">
-        <v>189</v>
+        <v>173</v>
       </c>
       <c r="C22" s="2" t="s">
-        <v>190</v>
+        <v>174</v>
       </c>
       <c r="D22" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E22" s="2" t="s">
         <v>9</v>
@@ -1449,22 +1858,22 @@
       <c r="F22" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G22" s="2" t="s">
-        <v>151</v>
+      <c r="G22" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="23" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
+      <c r="A23" s="2" t="s">
+        <v>304</v>
       </c>
       <c r="B23" s="2" t="s">
-        <v>191</v>
+        <v>175</v>
       </c>
       <c r="C23" s="2" t="s">
-        <v>192</v>
+        <v>176</v>
       </c>
       <c r="D23" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E23" s="2" t="s">
         <v>9</v>
@@ -1472,22 +1881,22 @@
       <c r="F23" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G23" s="2" t="s">
-        <v>154</v>
+      <c r="G23" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="24" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
+      <c r="A24" s="2" t="s">
+        <v>305</v>
       </c>
       <c r="B24" s="2" t="s">
-        <v>193</v>
+        <v>177</v>
       </c>
       <c r="C24" s="2" t="s">
-        <v>194</v>
+        <v>178</v>
       </c>
       <c r="D24" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E24" s="2" t="s">
         <v>9</v>
@@ -1495,22 +1904,22 @@
       <c r="F24" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G24" s="2" t="s">
-        <v>157</v>
+      <c r="G24" s="7" t="s">
+        <v>322</v>
       </c>
     </row>
     <row r="25" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
+      <c r="A25" s="2" t="s">
+        <v>306</v>
       </c>
       <c r="B25" s="2" t="s">
-        <v>195</v>
+        <v>179</v>
       </c>
       <c r="C25" s="2" t="s">
-        <v>196</v>
+        <v>180</v>
       </c>
       <c r="D25" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E25" s="2" t="s">
         <v>9</v>
@@ -1518,22 +1927,22 @@
       <c r="F25" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G25" s="2" t="s">
-        <v>160</v>
+      <c r="G25" s="7" t="s">
+        <v>321</v>
       </c>
     </row>
     <row r="26" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
+      <c r="A26" s="2" t="s">
+        <v>307</v>
       </c>
       <c r="B26" s="2" t="s">
-        <v>197</v>
+        <v>181</v>
       </c>
       <c r="C26" s="2" t="s">
-        <v>198</v>
+        <v>182</v>
       </c>
       <c r="D26" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E26" s="2" t="s">
         <v>9</v>
@@ -1541,22 +1950,22 @@
       <c r="F26" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G26" s="2" t="s">
-        <v>163</v>
+      <c r="G26" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="27" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>26</v>
+      <c r="A27" s="2" t="s">
+        <v>308</v>
       </c>
       <c r="B27" s="2" t="s">
-        <v>199</v>
+        <v>183</v>
       </c>
       <c r="C27" s="2" t="s">
-        <v>200</v>
+        <v>184</v>
       </c>
       <c r="D27" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E27" s="2" t="s">
         <v>9</v>
@@ -1564,22 +1973,22 @@
       <c r="F27" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G27" s="2" t="s">
-        <v>166</v>
+      <c r="G27" s="7" t="s">
+        <v>320</v>
       </c>
     </row>
     <row r="28" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>27</v>
+      <c r="A28" s="2" t="s">
+        <v>309</v>
       </c>
       <c r="B28" s="2" t="s">
-        <v>201</v>
+        <v>185</v>
       </c>
       <c r="C28" s="2" t="s">
-        <v>202</v>
+        <v>186</v>
       </c>
       <c r="D28" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E28" s="2" t="s">
         <v>9</v>
@@ -1587,22 +1996,22 @@
       <c r="F28" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G28" s="2" t="s">
-        <v>169</v>
+      <c r="G28" s="7" t="s">
+        <v>319</v>
       </c>
     </row>
     <row r="29" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>28</v>
+      <c r="A29" s="2" t="s">
+        <v>310</v>
       </c>
       <c r="B29" s="2" t="s">
-        <v>203</v>
+        <v>187</v>
       </c>
       <c r="C29" s="2" t="s">
-        <v>204</v>
+        <v>188</v>
       </c>
       <c r="D29" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E29" s="2" t="s">
         <v>9</v>
@@ -1610,22 +2019,22 @@
       <c r="F29" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G29" s="2" t="s">
-        <v>172</v>
+      <c r="G29" s="7" t="s">
+        <v>318</v>
       </c>
     </row>
     <row r="30" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
+      <c r="A30" s="2" t="s">
+        <v>311</v>
       </c>
       <c r="B30" s="2" t="s">
-        <v>205</v>
+        <v>189</v>
       </c>
       <c r="C30" s="2" t="s">
-        <v>206</v>
+        <v>190</v>
       </c>
       <c r="D30" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E30" s="2" t="s">
         <v>9</v>
@@ -1633,22 +2042,22 @@
       <c r="F30" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G30" s="2" t="s">
-        <v>175</v>
+      <c r="G30" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
     <row r="31" spans="1:7" ht="137.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>30</v>
+      <c r="A31" s="2" t="s">
+        <v>312</v>
       </c>
       <c r="B31" s="2" t="s">
-        <v>207</v>
+        <v>191</v>
       </c>
       <c r="C31" s="2" t="s">
-        <v>208</v>
+        <v>192</v>
       </c>
       <c r="D31" s="2" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="E31" s="2" t="s">
         <v>9</v>
@@ -1656,8 +2065,8 @@
       <c r="F31" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="G31" s="2" t="s">
-        <v>178</v>
+      <c r="G31" s="7" t="s">
+        <v>317</v>
       </c>
     </row>
   </sheetData>
@@ -1701,11 +2110,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{04F63D8A-001A-42C5-943F-A8797B090E62}">
   <dimension ref="A1:I16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:I16"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B16" sqref="B16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="29.453125" customWidth="1"/>
+    <col min="2" max="2" width="39.7265625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:9" ht="26" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -1736,12 +2149,12 @@
         <v>114</v>
       </c>
     </row>
-    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
+    <row r="2" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="2" t="s">
+        <v>223</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>115</v>
+        <v>323</v>
       </c>
       <c r="C2" s="2">
         <v>5</v>
@@ -1750,7 +2163,7 @@
         <v>16</v>
       </c>
       <c r="E2" s="2" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
       <c r="F2" s="2">
         <v>10</v>
@@ -1761,16 +2174,16 @@
       <c r="H2" s="4">
         <v>45657</v>
       </c>
-      <c r="I2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="I2" s="2" t="s">
+        <v>283</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="7" t="s">
+        <v>224</v>
       </c>
       <c r="B3" s="2" t="s">
-        <v>115</v>
+        <v>324</v>
       </c>
       <c r="C3" s="2">
         <v>5</v>
@@ -1779,7 +2192,7 @@
         <v>16</v>
       </c>
       <c r="E3" s="2" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
       <c r="F3" s="2">
         <v>10</v>
@@ -1790,16 +2203,16 @@
       <c r="H3" s="4">
         <v>45657</v>
       </c>
-      <c r="I3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="I3" s="2" t="s">
+        <v>284</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="7" t="s">
+        <v>225</v>
       </c>
       <c r="B4" s="2" t="s">
-        <v>115</v>
+        <v>325</v>
       </c>
       <c r="C4" s="2">
         <v>10</v>
@@ -1808,7 +2221,7 @@
         <v>16</v>
       </c>
       <c r="E4" s="2" t="s">
-        <v>118</v>
+        <v>117</v>
       </c>
       <c r="F4" s="2">
         <v>10</v>
@@ -1819,16 +2232,16 @@
       <c r="H4" s="4">
         <v>45657</v>
       </c>
-      <c r="I4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
+      <c r="I4" s="2" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="7" t="s">
+        <v>226</v>
       </c>
       <c r="B5" s="2" t="s">
-        <v>115</v>
+        <v>326</v>
       </c>
       <c r="C5" s="2">
         <v>5</v>
@@ -1837,7 +2250,7 @@
         <v>16</v>
       </c>
       <c r="E5" s="2" t="s">
-        <v>119</v>
+        <v>118</v>
       </c>
       <c r="F5" s="2">
         <v>10</v>
@@ -1848,16 +2261,16 @@
       <c r="H5" s="4">
         <v>45657</v>
       </c>
-      <c r="I5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="I5" s="2" t="s">
+        <v>286</v>
+      </c>
+    </row>
+    <row r="6" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="7" t="s">
+        <v>227</v>
       </c>
       <c r="B6" s="2" t="s">
-        <v>115</v>
+        <v>327</v>
       </c>
       <c r="C6" s="2">
         <v>20</v>
@@ -1866,7 +2279,7 @@
         <v>16</v>
       </c>
       <c r="E6" s="2" t="s">
-        <v>120</v>
+        <v>119</v>
       </c>
       <c r="F6" s="2">
         <v>10</v>
@@ -1877,16 +2290,16 @@
       <c r="H6" s="4">
         <v>45657</v>
       </c>
-      <c r="I6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
+      <c r="I6" s="2" t="s">
+        <v>287</v>
+      </c>
+    </row>
+    <row r="7" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="7" t="s">
+        <v>228</v>
       </c>
       <c r="B7" s="2" t="s">
-        <v>115</v>
+        <v>328</v>
       </c>
       <c r="C7" s="2">
         <v>10</v>
@@ -1895,7 +2308,7 @@
         <v>16</v>
       </c>
       <c r="E7" s="2" t="s">
-        <v>121</v>
+        <v>120</v>
       </c>
       <c r="F7" s="2">
         <v>10</v>
@@ -1906,16 +2319,16 @@
       <c r="H7" s="4">
         <v>45657</v>
       </c>
-      <c r="I7" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
+      <c r="I7" s="2" t="s">
+        <v>288</v>
+      </c>
+    </row>
+    <row r="8" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="2" t="s">
+        <v>229</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>115</v>
+        <v>329</v>
       </c>
       <c r="C8" s="2">
         <v>5</v>
@@ -1924,7 +2337,7 @@
         <v>16</v>
       </c>
       <c r="E8" s="2" t="s">
-        <v>122</v>
+        <v>121</v>
       </c>
       <c r="F8" s="2">
         <v>10</v>
@@ -1935,16 +2348,16 @@
       <c r="H8" s="4">
         <v>45657</v>
       </c>
-      <c r="I8" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
+      <c r="I8" s="2" t="s">
+        <v>289</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="2" t="s">
+        <v>230</v>
       </c>
       <c r="B9" s="2" t="s">
-        <v>115</v>
+        <v>330</v>
       </c>
       <c r="C9" s="2">
         <v>10</v>
@@ -1953,7 +2366,7 @@
         <v>16</v>
       </c>
       <c r="E9" s="2" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="F9" s="2">
         <v>10</v>
@@ -1964,16 +2377,16 @@
       <c r="H9" s="4">
         <v>45657</v>
       </c>
-      <c r="I9" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
+      <c r="I9" s="2" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="10" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="2" t="s">
+        <v>231</v>
       </c>
       <c r="B10" s="2" t="s">
-        <v>115</v>
+        <v>331</v>
       </c>
       <c r="C10" s="2">
         <v>5</v>
@@ -1982,7 +2395,7 @@
         <v>16</v>
       </c>
       <c r="E10" s="2" t="s">
-        <v>124</v>
+        <v>123</v>
       </c>
       <c r="F10" s="2">
         <v>10</v>
@@ -1993,16 +2406,16 @@
       <c r="H10" s="4">
         <v>45657</v>
       </c>
-      <c r="I10" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
+      <c r="I10" s="2" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="11" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="2" t="s">
+        <v>232</v>
       </c>
       <c r="B11" s="2" t="s">
-        <v>115</v>
+        <v>332</v>
       </c>
       <c r="C11" s="2">
         <v>20</v>
@@ -2011,7 +2424,7 @@
         <v>16</v>
       </c>
       <c r="E11" s="2" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="F11" s="2">
         <v>10</v>
@@ -2022,16 +2435,16 @@
       <c r="H11" s="4">
         <v>45657</v>
       </c>
-      <c r="I11" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
+      <c r="I11" s="2" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="12" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="7" t="s">
+        <v>233</v>
       </c>
       <c r="B12" s="2" t="s">
-        <v>115</v>
+        <v>333</v>
       </c>
       <c r="C12" s="2">
         <v>5</v>
@@ -2040,7 +2453,7 @@
         <v>16</v>
       </c>
       <c r="E12" s="2" t="s">
-        <v>126</v>
+        <v>125</v>
       </c>
       <c r="F12" s="2">
         <v>10</v>
@@ -2051,16 +2464,16 @@
       <c r="H12" s="4">
         <v>45657</v>
       </c>
-      <c r="I12" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
+      <c r="I12" s="2" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="13" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="7" t="s">
+        <v>234</v>
       </c>
       <c r="B13" s="2" t="s">
-        <v>115</v>
+        <v>334</v>
       </c>
       <c r="C13" s="2">
         <v>5</v>
@@ -2069,7 +2482,7 @@
         <v>16</v>
       </c>
       <c r="E13" s="2" t="s">
-        <v>127</v>
+        <v>126</v>
       </c>
       <c r="F13" s="2">
         <v>10</v>
@@ -2080,16 +2493,16 @@
       <c r="H13" s="4">
         <v>45657</v>
       </c>
-      <c r="I13" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
+      <c r="I13" s="2" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="14" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="7" t="s">
+        <v>235</v>
       </c>
       <c r="B14" s="2" t="s">
-        <v>115</v>
+        <v>335</v>
       </c>
       <c r="C14" s="2">
         <v>20</v>
@@ -2098,7 +2511,7 @@
         <v>16</v>
       </c>
       <c r="E14" s="2" t="s">
-        <v>128</v>
+        <v>127</v>
       </c>
       <c r="F14" s="2">
         <v>10</v>
@@ -2109,16 +2522,16 @@
       <c r="H14" s="4">
         <v>45657</v>
       </c>
-      <c r="I14" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
+      <c r="I14" s="2" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="15" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="2" t="s">
+        <v>236</v>
       </c>
       <c r="B15" s="2" t="s">
-        <v>115</v>
+        <v>336</v>
       </c>
       <c r="C15" s="2">
         <v>5</v>
@@ -2127,7 +2540,7 @@
         <v>16</v>
       </c>
       <c r="E15" s="2" t="s">
-        <v>129</v>
+        <v>128</v>
       </c>
       <c r="F15" s="2">
         <v>10</v>
@@ -2138,16 +2551,16 @@
       <c r="H15" s="4">
         <v>45657</v>
       </c>
-      <c r="I15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
+      <c r="I15" s="2" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="16" spans="1:9" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="2" t="s">
+        <v>237</v>
       </c>
       <c r="B16" s="2" t="s">
-        <v>115</v>
+        <v>337</v>
       </c>
       <c r="C16" s="2">
         <v>10</v>
@@ -2156,7 +2569,7 @@
         <v>16</v>
       </c>
       <c r="E16" s="2" t="s">
-        <v>130</v>
+        <v>129</v>
       </c>
       <c r="F16" s="2">
         <v>10</v>
@@ -2167,8 +2580,8 @@
       <c r="H16" s="4">
         <v>45657</v>
       </c>
-      <c r="I16" s="2">
-        <v>15</v>
+      <c r="I16" s="2" t="s">
+        <v>297</v>
       </c>
     </row>
   </sheetData>
@@ -2181,7 +2594,7 @@
   <dimension ref="A1:G31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:G31"/>
+      <selection activeCell="A2" sqref="A2:A31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
@@ -2210,8 +2623,8 @@
       </c>
     </row>
     <row r="2" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
+      <c r="A2" s="2" t="s">
+        <v>193</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>17</v>
@@ -2233,8 +2646,8 @@
       </c>
     </row>
     <row r="3" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="A3" s="2" t="s">
+        <v>194</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>20</v>
@@ -2256,8 +2669,8 @@
       </c>
     </row>
     <row r="4" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="A4" s="2" t="s">
+        <v>195</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>22</v>
@@ -2279,8 +2692,8 @@
       </c>
     </row>
     <row r="5" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
+      <c r="A5" s="2" t="s">
+        <v>196</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>24</v>
@@ -2302,8 +2715,8 @@
       </c>
     </row>
     <row r="6" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="A6" s="2" t="s">
+        <v>197</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>26</v>
@@ -2324,9 +2737,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
+    <row r="7" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="2" t="s">
+        <v>198</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>28</v>
@@ -2348,8 +2761,8 @@
       </c>
     </row>
     <row r="8" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
+      <c r="A8" s="2" t="s">
+        <v>199</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>30</v>
@@ -2371,8 +2784,8 @@
       </c>
     </row>
     <row r="9" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
+      <c r="A9" s="2" t="s">
+        <v>200</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>32</v>
@@ -2394,8 +2807,8 @@
       </c>
     </row>
     <row r="10" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
+      <c r="A10" s="2" t="s">
+        <v>201</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>34</v>
@@ -2417,8 +2830,8 @@
       </c>
     </row>
     <row r="11" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
+      <c r="A11" s="2" t="s">
+        <v>202</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>36</v>
@@ -2440,8 +2853,8 @@
       </c>
     </row>
     <row r="12" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
+      <c r="A12" s="2" t="s">
+        <v>203</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>38</v>
@@ -2463,8 +2876,8 @@
       </c>
     </row>
     <row r="13" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
+      <c r="A13" s="2" t="s">
+        <v>204</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>40</v>
@@ -2486,8 +2899,8 @@
       </c>
     </row>
     <row r="14" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
+      <c r="A14" s="2" t="s">
+        <v>205</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>42</v>
@@ -2509,8 +2922,8 @@
       </c>
     </row>
     <row r="15" spans="1:7" ht="62.5" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
+      <c r="A15" s="2" t="s">
+        <v>206</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>44</v>
@@ -2532,8 +2945,8 @@
       </c>
     </row>
     <row r="16" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
+      <c r="A16" s="2" t="s">
+        <v>207</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>46</v>
@@ -2554,9 +2967,9 @@
         <v>19</v>
       </c>
     </row>
-    <row r="17" spans="1:7" ht="25" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
+    <row r="17" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="2" t="s">
+        <v>208</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>48</v>
@@ -2578,8 +2991,8 @@
       </c>
     </row>
     <row r="18" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
+      <c r="A18" s="2" t="s">
+        <v>209</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>50</v>
@@ -2601,8 +3014,8 @@
       </c>
     </row>
     <row r="19" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
+      <c r="A19" s="2" t="s">
+        <v>210</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>52</v>
@@ -2624,8 +3037,8 @@
       </c>
     </row>
     <row r="20" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
+      <c r="A20" s="2" t="s">
+        <v>211</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>54</v>
@@ -2647,8 +3060,8 @@
       </c>
     </row>
     <row r="21" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
+      <c r="A21" s="2" t="s">
+        <v>212</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>56</v>
@@ -2670,8 +3083,8 @@
       </c>
     </row>
     <row r="22" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
+      <c r="A22" s="2" t="s">
+        <v>213</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>58</v>
@@ -2693,8 +3106,8 @@
       </c>
     </row>
     <row r="23" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
+      <c r="A23" s="2" t="s">
+        <v>214</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>60</v>
@@ -2716,8 +3129,8 @@
       </c>
     </row>
     <row r="24" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
+      <c r="A24" s="2" t="s">
+        <v>215</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>62</v>
@@ -2739,8 +3152,8 @@
       </c>
     </row>
     <row r="25" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
+      <c r="A25" s="2" t="s">
+        <v>216</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>64</v>
@@ -2762,8 +3175,8 @@
       </c>
     </row>
     <row r="26" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
+      <c r="A26" s="2" t="s">
+        <v>217</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>66</v>
@@ -2785,8 +3198,8 @@
       </c>
     </row>
     <row r="27" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>26</v>
+      <c r="A27" s="2" t="s">
+        <v>218</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>68</v>
@@ -2808,8 +3221,8 @@
       </c>
     </row>
     <row r="28" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>27</v>
+      <c r="A28" s="2" t="s">
+        <v>219</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>70</v>
@@ -2831,8 +3244,8 @@
       </c>
     </row>
     <row r="29" spans="1:7" ht="50" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>28</v>
+      <c r="A29" s="2" t="s">
+        <v>220</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>72</v>
@@ -2854,8 +3267,8 @@
       </c>
     </row>
     <row r="30" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
+      <c r="A30" s="2" t="s">
+        <v>221</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>74</v>
@@ -2877,8 +3290,8 @@
       </c>
     </row>
     <row r="31" spans="1:7" ht="37.5" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>30</v>
+      <c r="A31" s="2" t="s">
+        <v>222</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>76</v>
@@ -2909,10 +3322,15 @@
   <dimension ref="A1:D31"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:D31"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.5" x14ac:dyDescent="0.25"/>
+  <cols>
+    <col min="1" max="1" width="39" customWidth="1"/>
+    <col min="3" max="3" width="26.36328125" customWidth="1"/>
+    <col min="4" max="4" width="10.90625" customWidth="1"/>
+  </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
@@ -2928,424 +3346,424 @@
         <v>80</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A2" s="2">
-        <v>1</v>
+    <row r="2" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A2" s="6" t="s">
+        <v>253</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>81</v>
       </c>
-      <c r="C2" s="2">
-        <v>1</v>
-      </c>
-      <c r="D2" s="2">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A3" s="2">
-        <v>2</v>
+      <c r="C2" s="2" t="s">
+        <v>193</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A3" s="6" t="s">
+        <v>254</v>
       </c>
       <c r="B3" s="2" t="s">
         <v>82</v>
       </c>
-      <c r="C3" s="2">
-        <v>2</v>
-      </c>
-      <c r="D3" s="2">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A4" s="2">
-        <v>3</v>
+      <c r="C3" s="2" t="s">
+        <v>194</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A4" s="6" t="s">
+        <v>255</v>
       </c>
       <c r="B4" s="2" t="s">
         <v>83</v>
       </c>
-      <c r="C4" s="2">
-        <v>3</v>
-      </c>
-      <c r="D4" s="2">
-        <v>3</v>
-      </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A5" s="2">
-        <v>4</v>
+      <c r="C4" s="2" t="s">
+        <v>195</v>
+      </c>
+      <c r="D4" s="2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A5" s="6" t="s">
+        <v>256</v>
       </c>
       <c r="B5" s="2" t="s">
         <v>84</v>
       </c>
-      <c r="C5" s="2">
-        <v>4</v>
-      </c>
-      <c r="D5" s="2">
-        <v>4</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A6" s="2">
-        <v>5</v>
+      <c r="C5" s="2" t="s">
+        <v>196</v>
+      </c>
+      <c r="D5" s="2" t="s">
+        <v>226</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A6" s="6" t="s">
+        <v>257</v>
       </c>
       <c r="B6" s="2" t="s">
         <v>85</v>
       </c>
-      <c r="C6" s="2">
-        <v>5</v>
-      </c>
-      <c r="D6" s="2">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A7" s="2">
-        <v>6</v>
+      <c r="C6" s="2" t="s">
+        <v>197</v>
+      </c>
+      <c r="D6" s="2" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A7" s="6" t="s">
+        <v>258</v>
       </c>
       <c r="B7" s="2" t="s">
         <v>86</v>
       </c>
-      <c r="C7" s="2">
-        <v>6</v>
-      </c>
-      <c r="D7" s="2">
-        <v>6</v>
-      </c>
-    </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A8" s="2">
-        <v>7</v>
+      <c r="C7" s="2" t="s">
+        <v>198</v>
+      </c>
+      <c r="D7" s="2" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A8" s="6" t="s">
+        <v>259</v>
       </c>
       <c r="B8" s="2" t="s">
         <v>87</v>
       </c>
-      <c r="C8" s="2">
-        <v>7</v>
-      </c>
-      <c r="D8" s="2">
-        <v>7</v>
-      </c>
-    </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A9" s="2">
-        <v>8</v>
+      <c r="C8" s="2" t="s">
+        <v>199</v>
+      </c>
+      <c r="D8" s="2" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A9" s="6" t="s">
+        <v>260</v>
       </c>
       <c r="B9" s="2" t="s">
         <v>88</v>
       </c>
-      <c r="C9" s="2">
-        <v>8</v>
-      </c>
-      <c r="D9" s="2">
-        <v>8</v>
-      </c>
-    </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A10" s="2">
-        <v>9</v>
+      <c r="C9" s="2" t="s">
+        <v>200</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>230</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A10" s="6" t="s">
+        <v>261</v>
       </c>
       <c r="B10" s="2" t="s">
         <v>89</v>
       </c>
-      <c r="C10" s="2">
-        <v>9</v>
-      </c>
-      <c r="D10" s="2">
-        <v>9</v>
-      </c>
-    </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A11" s="2">
-        <v>10</v>
+      <c r="C10" s="2" t="s">
+        <v>201</v>
+      </c>
+      <c r="D10" s="2" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A11" s="6" t="s">
+        <v>262</v>
       </c>
       <c r="B11" s="2" t="s">
         <v>90</v>
       </c>
-      <c r="C11" s="2">
-        <v>10</v>
-      </c>
-      <c r="D11" s="2">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A12" s="2">
-        <v>11</v>
+      <c r="C11" s="2" t="s">
+        <v>202</v>
+      </c>
+      <c r="D11" s="2" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A12" s="6" t="s">
+        <v>263</v>
       </c>
       <c r="B12" s="2" t="s">
         <v>91</v>
       </c>
-      <c r="C12" s="2">
-        <v>11</v>
-      </c>
-      <c r="D12" s="2">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A13" s="2">
-        <v>12</v>
+      <c r="C12" s="2" t="s">
+        <v>203</v>
+      </c>
+      <c r="D12" s="2" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A13" s="6" t="s">
+        <v>264</v>
       </c>
       <c r="B13" s="2" t="s">
         <v>92</v>
       </c>
-      <c r="C13" s="2">
-        <v>12</v>
-      </c>
-      <c r="D13" s="2">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A14" s="2">
-        <v>13</v>
+      <c r="C13" s="2" t="s">
+        <v>204</v>
+      </c>
+      <c r="D13" s="2" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A14" s="6" t="s">
+        <v>265</v>
       </c>
       <c r="B14" s="2" t="s">
         <v>93</v>
       </c>
-      <c r="C14" s="2">
-        <v>13</v>
-      </c>
-      <c r="D14" s="2">
-        <v>13</v>
-      </c>
-    </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A15" s="2">
-        <v>14</v>
+      <c r="C14" s="2" t="s">
+        <v>205</v>
+      </c>
+      <c r="D14" s="2" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A15" s="6" t="s">
+        <v>266</v>
       </c>
       <c r="B15" s="2" t="s">
         <v>94</v>
       </c>
-      <c r="C15" s="2">
-        <v>14</v>
-      </c>
-      <c r="D15" s="2">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A16" s="2">
-        <v>15</v>
+      <c r="C15" s="2" t="s">
+        <v>206</v>
+      </c>
+      <c r="D15" s="2" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A16" s="6" t="s">
+        <v>267</v>
       </c>
       <c r="B16" s="2" t="s">
         <v>95</v>
       </c>
-      <c r="C16" s="2">
-        <v>15</v>
-      </c>
-      <c r="D16" s="2">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A17" s="2">
-        <v>16</v>
+      <c r="C16" s="2" t="s">
+        <v>207</v>
+      </c>
+      <c r="D16" s="2" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A17" s="6" t="s">
+        <v>268</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>96</v>
       </c>
-      <c r="C17" s="2">
-        <v>16</v>
-      </c>
-      <c r="D17" s="2">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A18" s="2">
-        <v>17</v>
+      <c r="C17" s="2" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="2" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A18" s="6" t="s">
+        <v>269</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>97</v>
       </c>
-      <c r="C18" s="2">
-        <v>17</v>
-      </c>
-      <c r="D18" s="2">
-        <v>17</v>
-      </c>
-    </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A19" s="2">
-        <v>18</v>
+      <c r="C18" s="2" t="s">
+        <v>209</v>
+      </c>
+      <c r="D18" s="2" t="s">
+        <v>239</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A19" s="6" t="s">
+        <v>270</v>
       </c>
       <c r="B19" s="2" t="s">
         <v>98</v>
       </c>
-      <c r="C19" s="2">
-        <v>18</v>
-      </c>
-      <c r="D19" s="2">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A20" s="2">
-        <v>19</v>
+      <c r="C19" s="2" t="s">
+        <v>210</v>
+      </c>
+      <c r="D19" s="2" t="s">
+        <v>240</v>
+      </c>
+    </row>
+    <row r="20" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A20" s="6" t="s">
+        <v>271</v>
       </c>
       <c r="B20" s="2" t="s">
         <v>99</v>
       </c>
-      <c r="C20" s="2">
-        <v>19</v>
-      </c>
-      <c r="D20" s="2">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A21" s="2">
-        <v>20</v>
+      <c r="C20" s="2" t="s">
+        <v>211</v>
+      </c>
+      <c r="D20" s="2" t="s">
+        <v>241</v>
+      </c>
+    </row>
+    <row r="21" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A21" s="6" t="s">
+        <v>272</v>
       </c>
       <c r="B21" s="2" t="s">
         <v>100</v>
       </c>
-      <c r="C21" s="2">
-        <v>20</v>
-      </c>
-      <c r="D21" s="2">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A22" s="2">
-        <v>21</v>
+      <c r="C21" s="2" t="s">
+        <v>212</v>
+      </c>
+      <c r="D21" s="2" t="s">
+        <v>242</v>
+      </c>
+    </row>
+    <row r="22" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A22" s="6" t="s">
+        <v>273</v>
       </c>
       <c r="B22" s="2" t="s">
         <v>101</v>
       </c>
-      <c r="C22" s="2">
-        <v>21</v>
-      </c>
-      <c r="D22" s="2">
-        <v>21</v>
-      </c>
-    </row>
-    <row r="23" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A23" s="2">
-        <v>22</v>
+      <c r="C22" s="2" t="s">
+        <v>213</v>
+      </c>
+      <c r="D22" s="2" t="s">
+        <v>243</v>
+      </c>
+    </row>
+    <row r="23" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A23" s="6" t="s">
+        <v>274</v>
       </c>
       <c r="B23" s="2" t="s">
         <v>102</v>
       </c>
-      <c r="C23" s="2">
-        <v>22</v>
-      </c>
-      <c r="D23" s="2">
-        <v>22</v>
-      </c>
-    </row>
-    <row r="24" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A24" s="2">
-        <v>23</v>
+      <c r="C23" s="2" t="s">
+        <v>214</v>
+      </c>
+      <c r="D23" s="2" t="s">
+        <v>244</v>
+      </c>
+    </row>
+    <row r="24" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A24" s="6" t="s">
+        <v>275</v>
       </c>
       <c r="B24" s="2" t="s">
         <v>103</v>
       </c>
-      <c r="C24" s="2">
-        <v>23</v>
-      </c>
-      <c r="D24" s="2">
-        <v>23</v>
-      </c>
-    </row>
-    <row r="25" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A25" s="2">
-        <v>24</v>
+      <c r="C24" s="2" t="s">
+        <v>215</v>
+      </c>
+      <c r="D24" s="2" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="25" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="6" t="s">
+        <v>276</v>
       </c>
       <c r="B25" s="2" t="s">
         <v>104</v>
       </c>
-      <c r="C25" s="2">
-        <v>24</v>
-      </c>
-      <c r="D25" s="2">
-        <v>24</v>
-      </c>
-    </row>
-    <row r="26" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A26" s="2">
-        <v>25</v>
+      <c r="C25" s="2" t="s">
+        <v>216</v>
+      </c>
+      <c r="D25" s="2" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="26" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A26" s="6" t="s">
+        <v>277</v>
       </c>
       <c r="B26" s="2" t="s">
         <v>105</v>
       </c>
-      <c r="C26" s="2">
-        <v>25</v>
-      </c>
-      <c r="D26" s="2">
-        <v>25</v>
-      </c>
-    </row>
-    <row r="27" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A27" s="2">
-        <v>26</v>
+      <c r="C26" s="2" t="s">
+        <v>217</v>
+      </c>
+      <c r="D26" s="2" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="27" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A27" s="6" t="s">
+        <v>278</v>
       </c>
       <c r="B27" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C27" s="2">
-        <v>26</v>
-      </c>
-      <c r="D27" s="2">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="28" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A28" s="2">
-        <v>27</v>
+      <c r="C27" s="2" t="s">
+        <v>218</v>
+      </c>
+      <c r="D27" s="2" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="28" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A28" s="6" t="s">
+        <v>279</v>
       </c>
       <c r="B28" s="2" t="s">
         <v>107</v>
       </c>
-      <c r="C28" s="2">
-        <v>27</v>
-      </c>
-      <c r="D28" s="2">
-        <v>27</v>
-      </c>
-    </row>
-    <row r="29" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A29" s="2">
-        <v>28</v>
+      <c r="C28" s="2" t="s">
+        <v>219</v>
+      </c>
+      <c r="D28" s="2" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="29" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A29" s="6" t="s">
+        <v>280</v>
       </c>
       <c r="B29" s="2" t="s">
         <v>108</v>
       </c>
-      <c r="C29" s="2">
-        <v>28</v>
-      </c>
-      <c r="D29" s="2">
-        <v>28</v>
-      </c>
-    </row>
-    <row r="30" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A30" s="2">
-        <v>29</v>
+      <c r="C29" s="2" t="s">
+        <v>220</v>
+      </c>
+      <c r="D29" s="2" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="30" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="6" t="s">
+        <v>281</v>
       </c>
       <c r="B30" s="2" t="s">
         <v>109</v>
       </c>
-      <c r="C30" s="2">
-        <v>29</v>
-      </c>
-      <c r="D30" s="2">
-        <v>29</v>
-      </c>
-    </row>
-    <row r="31" spans="1:4" x14ac:dyDescent="0.25">
-      <c r="A31" s="2">
-        <v>30</v>
+      <c r="C30" s="2" t="s">
+        <v>221</v>
+      </c>
+      <c r="D30" s="2" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="31" spans="1:4" ht="37.5" x14ac:dyDescent="0.25">
+      <c r="A31" s="6" t="s">
+        <v>282</v>
       </c>
       <c r="B31" s="2" t="s">
         <v>110</v>
       </c>
-      <c r="C31" s="2">
-        <v>30</v>
-      </c>
-      <c r="D31" s="2">
-        <v>30</v>
+      <c r="C31" s="2" t="s">
+        <v>222</v>
+      </c>
+      <c r="D31" s="2" t="s">
+        <v>252</v>
       </c>
     </row>
   </sheetData>

</xml_diff>